<commit_message>
Added GDP boost per % change in CDR for RAPID.
</commit_message>
<xml_diff>
--- a/SourceData/rapid/RPModData.xlsx
+++ b/SourceData/rapid/RPModData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\rapid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6620CAEC-8EB4-4BF5-A6C8-4091F993ED68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BB9F06-0118-4921-91E8-41D54B0AC2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{0B8C9F00-E09E-4752-9D15-A778954EC9EA}"/>
+    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" xr2:uid="{0B8C9F00-E09E-4752-9D15-A778954EC9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="CountryDefaultsDB" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="173">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -555,6 +555,9 @@
   <si>
     <t>&lt;Teacher Ratio (Secondary)&gt;</t>
   </si>
+  <si>
+    <t>&lt;GDP Boost per Percent Change in CDR&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -589,9 +592,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,15 +928,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E9563F-74D8-43BC-A614-79D5A72BD767}">
-  <dimension ref="A1:BW42"/>
+  <dimension ref="A1:BX42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BP1" sqref="BP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -1137,31 +1139,34 @@
         <v>135</v>
       </c>
       <c r="BP1" t="s">
+        <v>172</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>159</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>160</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>161</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>162</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>136</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>137</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>138</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1337,31 +1342,34 @@
         <v>49.808999999999997</v>
       </c>
       <c r="BP2">
+        <v>0.5</v>
+      </c>
+      <c r="BQ2">
         <v>43.685000000000002</v>
       </c>
-      <c r="BQ2">
+      <c r="BR2">
         <v>19.507000000000001</v>
       </c>
-      <c r="BR2">
+      <c r="BS2">
         <v>65.031000000000006</v>
       </c>
-      <c r="BS2">
+      <c r="BT2">
         <v>-0.9348333333333334</v>
       </c>
-      <c r="BT2">
+      <c r="BU2">
         <v>-1.06</v>
       </c>
-      <c r="BU2">
+      <c r="BV2">
         <v>-5.13</v>
       </c>
-      <c r="BV2">
+      <c r="BW2">
         <v>-12.690000000000001</v>
       </c>
-      <c r="BW2">
+      <c r="BX2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>24</v>
       </c>
@@ -1537,31 +1545,34 @@
         <v>76.372</v>
       </c>
       <c r="BP3">
+        <v>0.5</v>
+      </c>
+      <c r="BQ3">
         <v>21.684999999999999</v>
       </c>
-      <c r="BQ3">
+      <c r="BR3">
         <v>20.768000000000001</v>
       </c>
-      <c r="BR3">
+      <c r="BS3">
         <v>22.568999999999999</v>
       </c>
-      <c r="BS3">
+      <c r="BT3">
         <v>-1.5366666666666667E-2</v>
       </c>
-      <c r="BT3">
+      <c r="BU3">
         <v>-4</v>
       </c>
-      <c r="BU3">
+      <c r="BV3">
         <v>-8</v>
       </c>
-      <c r="BV3">
+      <c r="BW3">
         <v>-10</v>
       </c>
-      <c r="BW3">
+      <c r="BX3">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>50</v>
       </c>
@@ -1737,31 +1748,34 @@
         <v>58.328000000000003</v>
       </c>
       <c r="BP4">
+        <v>0.5</v>
+      </c>
+      <c r="BQ4">
         <v>29.998000000000001</v>
       </c>
-      <c r="BQ4">
+      <c r="BR4">
         <v>10.89</v>
       </c>
-      <c r="BR4">
+      <c r="BS4">
         <v>47.76</v>
       </c>
-      <c r="BS4">
+      <c r="BT4">
         <v>-1.0826666666666667</v>
       </c>
-      <c r="BT4">
+      <c r="BU4">
         <v>-2.4</v>
       </c>
-      <c r="BU4">
+      <c r="BV4">
         <v>-2.6</v>
       </c>
-      <c r="BV4">
+      <c r="BW4">
         <v>-2.8000000000000003</v>
       </c>
-      <c r="BW4">
+      <c r="BX4">
         <v>0.26</v>
       </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>204</v>
       </c>
@@ -1937,31 +1951,34 @@
         <v>62.741</v>
       </c>
       <c r="BP5">
+        <v>0.5</v>
+      </c>
+      <c r="BQ5">
         <v>15.196</v>
       </c>
-      <c r="BQ5">
+      <c r="BR5">
         <v>12.922000000000001</v>
       </c>
-      <c r="BR5">
+      <c r="BS5">
         <v>17.506</v>
       </c>
-      <c r="BS5">
+      <c r="BT5">
         <v>-1.9555666666666665</v>
       </c>
-      <c r="BT5">
+      <c r="BU5">
         <v>-3.29</v>
       </c>
-      <c r="BU5">
+      <c r="BV5">
         <v>-6.81</v>
       </c>
-      <c r="BV5">
+      <c r="BW5">
         <v>-8.58</v>
       </c>
-      <c r="BW5">
+      <c r="BX5">
         <v>0.27</v>
       </c>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>854</v>
       </c>
@@ -2137,31 +2154,34 @@
         <v>44.893000000000001</v>
       </c>
       <c r="BP6">
+        <v>0.5</v>
+      </c>
+      <c r="BQ6">
         <v>34.25</v>
       </c>
-      <c r="BQ6">
+      <c r="BR6">
         <v>27.038</v>
       </c>
-      <c r="BR6">
+      <c r="BS6">
         <v>39.517000000000003</v>
       </c>
-      <c r="BS6">
+      <c r="BT6">
         <v>-1.9608000000000001</v>
       </c>
-      <c r="BT6">
+      <c r="BU6">
         <v>-3.1</v>
       </c>
-      <c r="BU6">
+      <c r="BV6">
         <v>-6.5</v>
       </c>
-      <c r="BV6">
+      <c r="BW6">
         <v>-8.2000000000000011</v>
       </c>
-      <c r="BW6">
+      <c r="BX6">
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>108</v>
       </c>
@@ -2337,31 +2357,34 @@
         <v>78.557000000000002</v>
       </c>
       <c r="BP7">
+        <v>0.5</v>
+      </c>
+      <c r="BQ7">
         <v>11.167</v>
       </c>
-      <c r="BQ7">
+      <c r="BR7">
         <v>11.458</v>
       </c>
-      <c r="BR7">
+      <c r="BS7">
         <v>10.942</v>
       </c>
-      <c r="BS7">
+      <c r="BT7">
         <v>-0.80233333333333334</v>
       </c>
-      <c r="BT7">
+      <c r="BU7">
         <v>-2.6100000000000003</v>
       </c>
-      <c r="BU7">
+      <c r="BV7">
         <v>-5.6899999999999995</v>
       </c>
-      <c r="BV7">
+      <c r="BW7">
         <v>-7.23</v>
       </c>
-      <c r="BW7">
+      <c r="BX7">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>116</v>
       </c>
@@ -2537,31 +2560,34 @@
         <v>79.510000000000005</v>
       </c>
       <c r="BP8">
+        <v>0.5</v>
+      </c>
+      <c r="BQ8">
         <v>6.1879999999999997</v>
       </c>
-      <c r="BQ8">
+      <c r="BR8">
         <v>4.2699999999999996</v>
       </c>
-      <c r="BR8">
+      <c r="BS8">
         <v>8.1140000000000008</v>
       </c>
-      <c r="BS8">
+      <c r="BT8">
         <v>-2.1580000000000004</v>
       </c>
-      <c r="BT8">
+      <c r="BU8">
         <v>-1.25</v>
       </c>
-      <c r="BU8">
+      <c r="BV8">
         <v>-2.31</v>
       </c>
-      <c r="BV8">
+      <c r="BW8">
         <v>-3.38</v>
       </c>
-      <c r="BW8">
+      <c r="BX8">
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>120</v>
       </c>
@@ -2737,31 +2763,34 @@
         <v>3</v>
       </c>
       <c r="BP9">
+        <v>0.5</v>
+      </c>
+      <c r="BQ9">
         <v>23.222999999999999</v>
       </c>
-      <c r="BQ9">
+      <c r="BR9">
         <v>14.702999999999999</v>
       </c>
-      <c r="BR9">
+      <c r="BS9">
         <v>30.417999999999999</v>
       </c>
-      <c r="BS9">
+      <c r="BT9">
         <v>-0.87073333333333325</v>
       </c>
-      <c r="BT9">
+      <c r="BU9">
         <v>-3.44</v>
       </c>
-      <c r="BU9">
+      <c r="BV9">
         <v>-7.06</v>
       </c>
-      <c r="BV9">
+      <c r="BW9">
         <v>-8.8800000000000008</v>
       </c>
-      <c r="BW9">
+      <c r="BX9">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>384</v>
       </c>
@@ -2937,31 +2966,34 @@
         <v>64.683999999999997</v>
       </c>
       <c r="BP10">
+        <v>0.5</v>
+      </c>
+      <c r="BQ10">
         <v>18.777000000000001</v>
       </c>
-      <c r="BQ10">
+      <c r="BR10">
         <v>12.782999999999999</v>
       </c>
-      <c r="BR10">
+      <c r="BS10">
         <v>24.550999999999998</v>
       </c>
-      <c r="BS10">
+      <c r="BT10">
         <v>-2.4513333333333334</v>
       </c>
-      <c r="BT10">
+      <c r="BU10">
         <v>-0.75</v>
       </c>
-      <c r="BU10">
+      <c r="BV10">
         <v>-2.19</v>
       </c>
-      <c r="BV10">
+      <c r="BW10">
         <v>-3.63</v>
       </c>
-      <c r="BW10">
+      <c r="BX10">
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>180</v>
       </c>
@@ -3137,31 +3169,34 @@
         <v>63.44</v>
       </c>
       <c r="BP11">
+        <v>0.5</v>
+      </c>
+      <c r="BQ11">
         <v>31.373000000000001</v>
       </c>
-      <c r="BQ11">
+      <c r="BR11">
         <v>28.661000000000001</v>
       </c>
-      <c r="BR11">
+      <c r="BS11">
         <v>33.880000000000003</v>
       </c>
-      <c r="BS11">
+      <c r="BT11">
         <v>-0.26999999999999996</v>
       </c>
-      <c r="BT11">
+      <c r="BU11">
         <v>-3.51</v>
       </c>
-      <c r="BU11">
+      <c r="BV11">
         <v>-7.19</v>
       </c>
-      <c r="BV11">
+      <c r="BW11">
         <v>-9.0300000000000011</v>
       </c>
-      <c r="BW11">
+      <c r="BX11">
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>818</v>
       </c>
@@ -3337,31 +3372,34 @@
         <v>42.987000000000002</v>
       </c>
       <c r="BP12">
+        <v>0.5</v>
+      </c>
+      <c r="BQ12">
         <v>26.92</v>
       </c>
-      <c r="BQ12">
+      <c r="BR12">
         <v>15.833</v>
       </c>
-      <c r="BR12">
+      <c r="BS12">
         <v>40.116999999999997</v>
       </c>
-      <c r="BS12">
+      <c r="BT12">
         <v>-0.23016666666666666</v>
       </c>
-      <c r="BT12">
+      <c r="BU12">
         <v>-2.08</v>
       </c>
-      <c r="BU12">
+      <c r="BV12">
         <v>-5.35</v>
       </c>
-      <c r="BV12">
+      <c r="BW12">
         <v>-11.23</v>
       </c>
-      <c r="BW12">
+      <c r="BX12">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>231</v>
       </c>
@@ -3537,31 +3575,34 @@
         <v>68.253</v>
       </c>
       <c r="BP13">
+        <v>0.5</v>
+      </c>
+      <c r="BQ13">
         <v>17.529</v>
       </c>
-      <c r="BQ13">
+      <c r="BR13">
         <v>9.8689999999999998</v>
       </c>
-      <c r="BR13">
+      <c r="BS13">
         <v>24.875</v>
       </c>
-      <c r="BS13">
+      <c r="BT13">
         <v>0</v>
       </c>
-      <c r="BT13">
+      <c r="BU13">
         <v>-3.3300000000000005</v>
       </c>
-      <c r="BU13">
+      <c r="BV13">
         <v>-6.88</v>
       </c>
-      <c r="BV13">
+      <c r="BW13">
         <v>-8.6499999999999986</v>
       </c>
-      <c r="BW13">
+      <c r="BX13">
         <v>0.33999999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>288</v>
       </c>
@@ -3737,31 +3778,34 @@
         <v>71.34</v>
       </c>
       <c r="BP14">
+        <v>0.5</v>
+      </c>
+      <c r="BQ14">
         <v>27.734000000000002</v>
       </c>
-      <c r="BQ14">
+      <c r="BR14">
         <v>25.393999999999998</v>
       </c>
-      <c r="BR14">
+      <c r="BS14">
         <v>29.916</v>
       </c>
-      <c r="BS14">
+      <c r="BT14">
         <v>-2.5381</v>
       </c>
-      <c r="BT14">
+      <c r="BU14">
         <v>-3.4000000000000004</v>
       </c>
-      <c r="BU14">
+      <c r="BV14">
         <v>-7.0000000000000009</v>
       </c>
-      <c r="BV14">
+      <c r="BW14">
         <v>-8.7999999999999989</v>
       </c>
-      <c r="BW14">
+      <c r="BX14">
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>320</v>
       </c>
@@ -3937,31 +3981,34 @@
         <v>60.241</v>
       </c>
       <c r="BP15">
+        <v>0.5</v>
+      </c>
+      <c r="BQ15">
         <v>29.552</v>
       </c>
-      <c r="BQ15">
+      <c r="BR15">
         <v>12.897</v>
       </c>
-      <c r="BR15">
+      <c r="BS15">
         <v>44.347000000000001</v>
       </c>
-      <c r="BS15">
+      <c r="BT15">
         <v>-0.10626666666666666</v>
       </c>
-      <c r="BT15">
+      <c r="BU15">
         <v>-2.8000000000000003</v>
       </c>
-      <c r="BU15">
+      <c r="BV15">
         <v>-6</v>
       </c>
-      <c r="BV15">
+      <c r="BW15">
         <v>-7.6</v>
       </c>
-      <c r="BW15">
+      <c r="BX15">
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>324</v>
       </c>
@@ -4137,31 +4184,34 @@
         <v>52.878999999999998</v>
       </c>
       <c r="BP16">
+        <v>0.5</v>
+      </c>
+      <c r="BQ16">
         <v>34.301000000000002</v>
       </c>
-      <c r="BQ16">
+      <c r="BR16">
         <v>24.844999999999999</v>
       </c>
-      <c r="BR16">
+      <c r="BS16">
         <v>41.491999999999997</v>
       </c>
-      <c r="BS16">
+      <c r="BT16">
         <v>-0.81636666666666668</v>
       </c>
-      <c r="BT16">
+      <c r="BU16">
         <v>-1</v>
       </c>
-      <c r="BU16">
+      <c r="BV16">
         <v>-2.25</v>
       </c>
-      <c r="BV16">
+      <c r="BW16">
         <v>-3.5000000000000004</v>
       </c>
-      <c r="BW16">
+      <c r="BX16">
         <v>0.27</v>
       </c>
     </row>
-    <row r="17" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>332</v>
       </c>
@@ -4336,8 +4386,8 @@
       <c r="BO17" t="s">
         <v>3</v>
       </c>
-      <c r="BP17" t="s">
-        <v>3</v>
+      <c r="BP17">
+        <v>0.5</v>
       </c>
       <c r="BQ17" t="s">
         <v>3</v>
@@ -4345,23 +4395,26 @@
       <c r="BR17" t="s">
         <v>3</v>
       </c>
-      <c r="BS17">
+      <c r="BS17" t="s">
+        <v>3</v>
+      </c>
+      <c r="BT17">
         <v>-1.1048333333333333</v>
       </c>
-      <c r="BT17">
+      <c r="BU17">
         <v>-3.0300000000000002</v>
       </c>
-      <c r="BU17">
+      <c r="BV17">
         <v>-6.38</v>
       </c>
-      <c r="BV17">
+      <c r="BW17">
         <v>-8.0500000000000007</v>
       </c>
-      <c r="BW17">
+      <c r="BX17">
         <v>0.27</v>
       </c>
     </row>
-    <row r="18" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>356</v>
       </c>
@@ -4537,31 +4590,34 @@
         <v>52.353999999999999</v>
       </c>
       <c r="BP18">
+        <v>0.5</v>
+      </c>
+      <c r="BQ18">
         <v>23.494</v>
       </c>
-      <c r="BQ18">
+      <c r="BR18">
         <v>10.231</v>
       </c>
-      <c r="BR18">
+      <c r="BS18">
         <v>38.127000000000002</v>
       </c>
-      <c r="BS18">
+      <c r="BT18">
         <v>-1.1015333333333333</v>
       </c>
-      <c r="BT18">
+      <c r="BU18">
         <v>-2.25</v>
       </c>
-      <c r="BU18">
+      <c r="BV18">
         <v>-2.56</v>
       </c>
-      <c r="BV18">
+      <c r="BW18">
         <v>-2.88</v>
       </c>
-      <c r="BW18">
+      <c r="BX18">
         <v>0.26</v>
       </c>
     </row>
-    <row r="19" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>400</v>
       </c>
@@ -4737,31 +4793,34 @@
         <v>38.67</v>
       </c>
       <c r="BP19">
+        <v>0.5</v>
+      </c>
+      <c r="BQ19">
         <v>31.495000000000001</v>
       </c>
-      <c r="BQ19">
+      <c r="BR19">
         <v>27.486000000000001</v>
       </c>
-      <c r="BR19">
+      <c r="BS19">
         <v>36.055</v>
       </c>
-      <c r="BS19">
+      <c r="BT19">
         <v>-4.8766666666666666E-2</v>
       </c>
-      <c r="BT19">
+      <c r="BU19">
         <v>-2.98</v>
       </c>
-      <c r="BU19">
+      <c r="BV19">
         <v>-5.55</v>
       </c>
-      <c r="BV19">
+      <c r="BW19">
         <v>-9.93</v>
       </c>
-      <c r="BW19">
+      <c r="BX19">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>404</v>
       </c>
@@ -4964,31 +5023,34 @@
         <v>67.462000000000003</v>
       </c>
       <c r="BP20">
+        <v>0.5</v>
+      </c>
+      <c r="BQ20">
         <v>18.733000000000001</v>
       </c>
-      <c r="BQ20">
+      <c r="BR20">
         <v>12.206</v>
       </c>
-      <c r="BR20">
+      <c r="BS20">
         <v>24.966999999999999</v>
       </c>
-      <c r="BS20">
+      <c r="BT20">
         <v>-5.6599999999999998E-2</v>
       </c>
-      <c r="BT20">
+      <c r="BU20">
         <v>-4</v>
       </c>
-      <c r="BU20">
+      <c r="BV20">
         <v>-8</v>
       </c>
-      <c r="BV20">
+      <c r="BW20">
         <v>-10</v>
       </c>
-      <c r="BW20">
+      <c r="BX20">
         <v>0.31</v>
       </c>
     </row>
-    <row r="21" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>430</v>
       </c>
@@ -5164,31 +5226,34 @@
         <v>46.587000000000003</v>
       </c>
       <c r="BP21">
+        <v>0.5</v>
+      </c>
+      <c r="BQ21">
         <v>40.780999999999999</v>
       </c>
-      <c r="BQ21">
+      <c r="BR21">
         <v>39.854999999999997</v>
       </c>
-      <c r="BR21">
+      <c r="BS21">
         <v>41.554000000000002</v>
       </c>
-      <c r="BS21">
+      <c r="BT21">
         <v>-1.3322000000000001</v>
       </c>
-      <c r="BT21">
+      <c r="BU21">
         <v>-0.85000000000000009</v>
       </c>
-      <c r="BU21">
+      <c r="BV21">
         <v>-2.21</v>
       </c>
-      <c r="BV21">
+      <c r="BW21">
         <v>-3.58</v>
       </c>
-      <c r="BW21">
+      <c r="BX21">
         <v>0.27</v>
       </c>
     </row>
-    <row r="22" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>450</v>
       </c>
@@ -5364,31 +5429,34 @@
         <v>86.381</v>
       </c>
       <c r="BP22">
+        <v>0.5</v>
+      </c>
+      <c r="BQ22">
         <v>24.488</v>
       </c>
-      <c r="BQ22">
+      <c r="BR22">
         <v>18.661999999999999</v>
       </c>
-      <c r="BR22">
+      <c r="BS22">
         <v>30.102</v>
       </c>
-      <c r="BS22">
+      <c r="BT22">
         <v>-0.83770000000000011</v>
       </c>
-      <c r="BT22">
+      <c r="BU22">
         <v>-1.9</v>
       </c>
-      <c r="BU22">
+      <c r="BV22">
         <v>-2.48</v>
       </c>
-      <c r="BV22">
+      <c r="BW22">
         <v>-3.05</v>
       </c>
-      <c r="BW22">
+      <c r="BX22">
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>454</v>
       </c>
@@ -5564,31 +5632,34 @@
         <v>68.27</v>
       </c>
       <c r="BP23">
+        <v>0.5</v>
+      </c>
+      <c r="BQ23">
         <v>19.41</v>
       </c>
-      <c r="BQ23">
+      <c r="BR23">
         <v>13.664999999999999</v>
       </c>
-      <c r="BR23">
+      <c r="BS23">
         <v>24.887</v>
       </c>
-      <c r="BS23">
+      <c r="BT23">
         <v>-0.51616666666666666</v>
       </c>
-      <c r="BT23">
+      <c r="BU23">
         <v>-3.0300000000000002</v>
       </c>
-      <c r="BU23">
+      <c r="BV23">
         <v>-6.38</v>
       </c>
-      <c r="BV23">
+      <c r="BW23">
         <v>-8.0500000000000007</v>
       </c>
-      <c r="BW23">
+      <c r="BX23">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>466</v>
       </c>
@@ -5764,31 +5835,34 @@
         <v>65.915999999999997</v>
       </c>
       <c r="BP24">
+        <v>0.5</v>
+      </c>
+      <c r="BQ24">
         <v>30.861999999999998</v>
       </c>
-      <c r="BQ24">
+      <c r="BR24">
         <v>15.21</v>
       </c>
-      <c r="BR24">
+      <c r="BS24">
         <v>43.316000000000003</v>
       </c>
-      <c r="BS24">
+      <c r="BT24">
         <v>-1.3322000000000001</v>
       </c>
-      <c r="BT24">
+      <c r="BU24">
         <v>-3.36</v>
       </c>
-      <c r="BU24">
+      <c r="BV24">
         <v>-6.94</v>
       </c>
-      <c r="BV24">
+      <c r="BW24">
         <v>-8.73</v>
       </c>
-      <c r="BW24">
+      <c r="BX24">
         <v>0.27</v>
       </c>
     </row>
-    <row r="25" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>478</v>
       </c>
@@ -5964,31 +6038,34 @@
         <v>45.466999999999999</v>
       </c>
       <c r="BP25">
+        <v>0.5</v>
+      </c>
+      <c r="BQ25">
         <v>44.085000000000001</v>
       </c>
-      <c r="BQ25">
+      <c r="BR25">
         <v>32.026000000000003</v>
       </c>
-      <c r="BR25">
+      <c r="BS25">
         <v>54.847000000000001</v>
       </c>
-      <c r="BS25">
+      <c r="BT25">
         <v>-1.3322000000000001</v>
       </c>
-      <c r="BT25">
+      <c r="BU25">
         <v>-0.85000000000000009</v>
       </c>
-      <c r="BU25">
+      <c r="BV25">
         <v>-2.21</v>
       </c>
-      <c r="BV25">
+      <c r="BW25">
         <v>-3.58</v>
       </c>
-      <c r="BW25">
+      <c r="BX25">
         <v>0.27</v>
       </c>
     </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>508</v>
       </c>
@@ -6163,8 +6240,8 @@
       <c r="BO26">
         <v>79.052999999999997</v>
       </c>
-      <c r="BP26" t="s">
-        <v>3</v>
+      <c r="BP26">
+        <v>0.5</v>
       </c>
       <c r="BQ26" t="s">
         <v>3</v>
@@ -6172,23 +6249,26 @@
       <c r="BR26" t="s">
         <v>3</v>
       </c>
-      <c r="BS26">
+      <c r="BS26" t="s">
+        <v>3</v>
+      </c>
+      <c r="BT26">
         <v>-0.90426666666666655</v>
       </c>
-      <c r="BT26">
+      <c r="BU26">
         <v>-2.6100000000000003</v>
       </c>
-      <c r="BU26">
+      <c r="BV26">
         <v>-5.6899999999999995</v>
       </c>
-      <c r="BV26">
+      <c r="BW26">
         <v>-7.23</v>
       </c>
-      <c r="BW26">
+      <c r="BX26">
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>524</v>
       </c>
@@ -6364,31 +6444,34 @@
         <v>39.914999999999999</v>
       </c>
       <c r="BP27">
+        <v>0.5</v>
+      </c>
+      <c r="BQ27">
         <v>34.762999999999998</v>
       </c>
-      <c r="BQ27">
+      <c r="BR27">
         <v>21.155999999999999</v>
       </c>
-      <c r="BR27">
+      <c r="BS27">
         <v>45.817</v>
       </c>
-      <c r="BS27">
+      <c r="BT27">
         <v>-0.37036666666666662</v>
       </c>
-      <c r="BT27">
+      <c r="BU27">
         <v>-2.8000000000000003</v>
       </c>
-      <c r="BU27">
+      <c r="BV27">
         <v>-2.7</v>
       </c>
-      <c r="BV27">
+      <c r="BW27">
         <v>-2.6</v>
       </c>
-      <c r="BW27">
+      <c r="BX27">
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>562</v>
       </c>
@@ -6564,31 +6647,34 @@
         <v>72.911000000000001</v>
       </c>
       <c r="BP28">
+        <v>0.5</v>
+      </c>
+      <c r="BQ28">
         <v>15.67</v>
       </c>
-      <c r="BQ28">
+      <c r="BR28">
         <v>8.8789999999999996</v>
       </c>
-      <c r="BR28">
+      <c r="BS28">
         <v>21.998999999999999</v>
       </c>
-      <c r="BS28">
+      <c r="BT28">
         <v>-1.3322000000000001</v>
       </c>
-      <c r="BT28">
+      <c r="BU28">
         <v>-0.85000000000000009</v>
       </c>
-      <c r="BU28">
+      <c r="BV28">
         <v>-2.21</v>
       </c>
-      <c r="BV28">
+      <c r="BW28">
         <v>-3.58</v>
       </c>
-      <c r="BW28">
+      <c r="BX28">
         <v>0.27</v>
       </c>
     </row>
-    <row r="29" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>566</v>
       </c>
@@ -6764,31 +6850,34 @@
         <v>81.27</v>
       </c>
       <c r="BP29">
+        <v>0.5</v>
+      </c>
+      <c r="BQ29">
         <v>13.86</v>
       </c>
-      <c r="BQ29">
+      <c r="BR29">
         <v>8.82</v>
       </c>
-      <c r="BR29">
+      <c r="BS29">
         <v>18.922000000000001</v>
       </c>
-      <c r="BS29">
+      <c r="BT29">
         <v>-2.7365333333333335</v>
       </c>
-      <c r="BT29">
+      <c r="BU29">
         <v>-3.3300000000000005</v>
       </c>
-      <c r="BU29">
+      <c r="BV29">
         <v>-6.88</v>
       </c>
-      <c r="BV29">
+      <c r="BW29">
         <v>-8.6499999999999986</v>
       </c>
-      <c r="BW29">
+      <c r="BX29">
         <v>0.27</v>
       </c>
     </row>
-    <row r="30" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>586</v>
       </c>
@@ -6964,31 +7053,34 @@
         <v>52.73</v>
       </c>
       <c r="BP30">
+        <v>0.5</v>
+      </c>
+      <c r="BQ30">
         <v>34.564</v>
       </c>
-      <c r="BQ30">
+      <c r="BR30">
         <v>13.59</v>
       </c>
-      <c r="BR30">
+      <c r="BS30">
         <v>56.417000000000002</v>
       </c>
-      <c r="BS30">
+      <c r="BT30">
         <v>-0.40556666666666669</v>
       </c>
-      <c r="BT30">
+      <c r="BU30">
         <v>-2.75</v>
       </c>
-      <c r="BU30">
+      <c r="BV30">
         <v>-5.5</v>
       </c>
-      <c r="BV30">
+      <c r="BW30">
         <v>-10.25</v>
       </c>
-      <c r="BW30">
+      <c r="BX30">
         <v>0.26</v>
       </c>
     </row>
-    <row r="31" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>608</v>
       </c>
@@ -7164,31 +7256,34 @@
         <v>56.470999999999997</v>
       </c>
       <c r="BP31">
+        <v>0.5</v>
+      </c>
+      <c r="BQ31">
         <v>12.756</v>
       </c>
-      <c r="BQ31">
+      <c r="BR31">
         <v>10.201000000000001</v>
       </c>
-      <c r="BR31">
+      <c r="BS31">
         <v>15.436</v>
       </c>
-      <c r="BS31">
+      <c r="BT31">
         <v>-1.5609999999999999</v>
       </c>
-      <c r="BT31">
+      <c r="BU31">
         <v>-1.3</v>
       </c>
-      <c r="BU31">
+      <c r="BV31">
         <v>-2.33</v>
       </c>
-      <c r="BV31">
+      <c r="BW31">
         <v>-3.35</v>
       </c>
-      <c r="BW31">
+      <c r="BX31">
         <v>0.27</v>
       </c>
     </row>
-    <row r="32" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>646</v>
       </c>
@@ -7364,31 +7459,34 @@
         <v>60.161999999999999</v>
       </c>
       <c r="BP32">
+        <v>0.5</v>
+      </c>
+      <c r="BQ32">
         <v>27.922999999999998</v>
       </c>
-      <c r="BQ32">
+      <c r="BR32">
         <v>24.498000000000001</v>
       </c>
-      <c r="BR32">
+      <c r="BS32">
         <v>31.27</v>
       </c>
-      <c r="BS32">
+      <c r="BT32">
         <v>0</v>
       </c>
-      <c r="BT32">
+      <c r="BU32">
         <v>-3.85</v>
       </c>
-      <c r="BU32">
+      <c r="BV32">
         <v>-7.75</v>
       </c>
-      <c r="BV32">
+      <c r="BW32">
         <v>-9.7000000000000011</v>
       </c>
-      <c r="BW32">
+      <c r="BX32">
         <v>0.33</v>
       </c>
     </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>686</v>
       </c>
@@ -7564,31 +7662,34 @@
         <v>50.712000000000003</v>
       </c>
       <c r="BP33">
+        <v>0.5</v>
+      </c>
+      <c r="BQ33">
         <v>33.033999999999999</v>
       </c>
-      <c r="BQ33">
+      <c r="BR33">
         <v>22.216000000000001</v>
       </c>
-      <c r="BR33">
+      <c r="BS33">
         <v>42.424999999999997</v>
       </c>
-      <c r="BS33">
+      <c r="BT33">
         <v>-1.2255333333333334</v>
       </c>
-      <c r="BT33">
+      <c r="BU33">
         <v>-1.4500000000000002</v>
       </c>
-      <c r="BU33">
+      <c r="BV33">
         <v>-2.36</v>
       </c>
-      <c r="BV33">
+      <c r="BW33">
         <v>-3.2800000000000002</v>
       </c>
-      <c r="BW33">
+      <c r="BX33">
         <v>0.26</v>
       </c>
     </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>694</v>
       </c>
@@ -7764,31 +7865,34 @@
         <v>53.911999999999999</v>
       </c>
       <c r="BP34">
+        <v>0.5</v>
+      </c>
+      <c r="BQ34">
         <v>33.167000000000002</v>
       </c>
-      <c r="BQ34">
+      <c r="BR34">
         <v>31.227</v>
       </c>
-      <c r="BR34">
+      <c r="BS34">
         <v>34.813000000000002</v>
       </c>
-      <c r="BS34">
+      <c r="BT34">
         <v>-1.3322000000000001</v>
       </c>
-      <c r="BT34">
+      <c r="BU34">
         <v>-0.85000000000000009</v>
       </c>
-      <c r="BU34">
+      <c r="BV34">
         <v>-2.21</v>
       </c>
-      <c r="BV34">
+      <c r="BW34">
         <v>-3.58</v>
       </c>
-      <c r="BW34">
+      <c r="BX34">
         <v>0.27</v>
       </c>
     </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>728</v>
       </c>
@@ -7963,8 +8067,8 @@
       <c r="BO35" t="s">
         <v>3</v>
       </c>
-      <c r="BP35" t="s">
-        <v>3</v>
+      <c r="BP35">
+        <v>0.5</v>
       </c>
       <c r="BQ35" t="s">
         <v>3</v>
@@ -7972,23 +8076,26 @@
       <c r="BR35" t="s">
         <v>3</v>
       </c>
-      <c r="BS35">
+      <c r="BS35" t="s">
+        <v>3</v>
+      </c>
+      <c r="BT35">
         <v>-4.1400000000000006E-2</v>
       </c>
-      <c r="BT35">
+      <c r="BU35">
         <v>-1.49</v>
       </c>
-      <c r="BU35">
+      <c r="BV35">
         <v>-3.81</v>
       </c>
-      <c r="BV35">
+      <c r="BW35">
         <v>-4.9799999999999995</v>
       </c>
-      <c r="BW35">
+      <c r="BX35">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>834</v>
       </c>
@@ -8164,31 +8271,34 @@
         <v>80.391999999999996</v>
       </c>
       <c r="BP36">
+        <v>0.5</v>
+      </c>
+      <c r="BQ36">
         <v>14.353</v>
       </c>
-      <c r="BQ36">
+      <c r="BR36">
         <v>9.06</v>
       </c>
-      <c r="BR36">
+      <c r="BS36">
         <v>19.286000000000001</v>
       </c>
-      <c r="BS36">
+      <c r="BT36">
         <v>-0.47716666666666663</v>
       </c>
-      <c r="BT36">
+      <c r="BU36">
         <v>-3.51</v>
       </c>
-      <c r="BU36">
+      <c r="BV36">
         <v>-7.19</v>
       </c>
-      <c r="BV36">
+      <c r="BW36">
         <v>-9.0300000000000011</v>
       </c>
-      <c r="BW36">
+      <c r="BX36">
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>626</v>
       </c>
@@ -8364,31 +8474,34 @@
         <v>34.625</v>
       </c>
       <c r="BP37">
+        <v>0.5</v>
+      </c>
+      <c r="BQ37">
         <v>29.122</v>
       </c>
-      <c r="BQ37">
+      <c r="BR37">
         <v>29.053000000000001</v>
       </c>
-      <c r="BR37">
+      <c r="BS37">
         <v>29.192</v>
       </c>
-      <c r="BS37">
+      <c r="BT37">
         <v>-2.1580000000000004</v>
       </c>
-      <c r="BT37">
+      <c r="BU37">
         <v>-3.06</v>
       </c>
-      <c r="BU37">
+      <c r="BV37">
         <v>-6.4399999999999995</v>
       </c>
-      <c r="BV37">
+      <c r="BW37">
         <v>-8.129999999999999</v>
       </c>
-      <c r="BW37">
+      <c r="BX37">
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>768</v>
       </c>
@@ -8564,31 +8677,34 @@
         <v>75.251999999999995</v>
       </c>
       <c r="BP38">
+        <v>0.5</v>
+      </c>
+      <c r="BQ38">
         <v>13.250999999999999</v>
       </c>
-      <c r="BQ38">
+      <c r="BR38">
         <v>10.509</v>
       </c>
-      <c r="BR38">
+      <c r="BS38">
         <v>15.775</v>
       </c>
-      <c r="BS38">
+      <c r="BT38">
         <v>-2.2635999999999998</v>
       </c>
-      <c r="BT38">
+      <c r="BU38">
         <v>-3.36</v>
       </c>
-      <c r="BU38">
+      <c r="BV38">
         <v>-6.94</v>
       </c>
-      <c r="BV38">
+      <c r="BW38">
         <v>-8.73</v>
       </c>
-      <c r="BW38">
+      <c r="BX38">
         <v>0.27999999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>800</v>
       </c>
@@ -8764,31 +8880,34 @@
         <v>79.201999999999998</v>
       </c>
       <c r="BP39">
+        <v>0.5</v>
+      </c>
+      <c r="BQ39">
         <v>13.805</v>
       </c>
-      <c r="BQ39">
+      <c r="BR39">
         <v>9.4049999999999994</v>
       </c>
-      <c r="BR39">
+      <c r="BS39">
         <v>17.788</v>
       </c>
-      <c r="BS39">
+      <c r="BT39">
         <v>-0.11066666666666666</v>
       </c>
-      <c r="BT39">
+      <c r="BU39">
         <v>-3.8899999999999997</v>
       </c>
-      <c r="BU39">
+      <c r="BV39">
         <v>-7.8100000000000005</v>
       </c>
-      <c r="BV39">
+      <c r="BW39">
         <v>-9.7799999999999994</v>
       </c>
-      <c r="BW39">
+      <c r="BX39">
         <v>0.31</v>
       </c>
     </row>
-    <row r="40" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>887</v>
       </c>
@@ -8963,8 +9082,8 @@
       <c r="BO40" t="s">
         <v>3</v>
       </c>
-      <c r="BP40" t="s">
-        <v>3</v>
+      <c r="BP40">
+        <v>0.5</v>
       </c>
       <c r="BQ40" t="s">
         <v>3</v>
@@ -8972,23 +9091,26 @@
       <c r="BR40" t="s">
         <v>3</v>
       </c>
-      <c r="BS40">
+      <c r="BS40" t="s">
+        <v>3</v>
+      </c>
+      <c r="BT40">
         <v>-9.5599999999999991E-2</v>
       </c>
-      <c r="BT40">
+      <c r="BU40">
         <v>-2.98</v>
       </c>
-      <c r="BU40">
+      <c r="BV40">
         <v>-5.55</v>
       </c>
-      <c r="BV40">
+      <c r="BW40">
         <v>-9.93</v>
       </c>
-      <c r="BW40">
+      <c r="BX40">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>894</v>
       </c>
@@ -9164,31 +9286,34 @@
         <v>60.119</v>
       </c>
       <c r="BP41">
+        <v>0.5</v>
+      </c>
+      <c r="BQ41">
         <v>29.367999999999999</v>
       </c>
-      <c r="BQ41">
+      <c r="BR41">
         <v>25.247</v>
       </c>
-      <c r="BR41">
+      <c r="BS41">
         <v>33.469000000000001</v>
       </c>
-      <c r="BS41">
+      <c r="BT41">
         <v>-0.15919999999999998</v>
       </c>
-      <c r="BT41">
+      <c r="BU41">
         <v>-3.0300000000000002</v>
       </c>
-      <c r="BU41">
+      <c r="BV41">
         <v>-6.38</v>
       </c>
-      <c r="BV41">
+      <c r="BW41">
         <v>-8.0500000000000007</v>
       </c>
-      <c r="BW41">
+      <c r="BX41">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>716</v>
       </c>
@@ -9364,27 +9489,30 @@
         <v>65.397999999999996</v>
       </c>
       <c r="BP42">
+        <v>0.5</v>
+      </c>
+      <c r="BQ42">
         <v>32.235999999999997</v>
       </c>
-      <c r="BQ42">
+      <c r="BR42">
         <v>26.635000000000002</v>
       </c>
-      <c r="BR42">
+      <c r="BS42">
         <v>37.689</v>
       </c>
-      <c r="BS42">
+      <c r="BT42">
         <v>-4.2999999999999997E-2</v>
       </c>
-      <c r="BT42">
+      <c r="BU42">
         <v>-2.6100000000000003</v>
       </c>
-      <c r="BU42">
+      <c r="BV42">
         <v>-5.6899999999999995</v>
       </c>
-      <c r="BV42">
+      <c r="BW42">
         <v>-7.23</v>
       </c>
-      <c r="BW42">
+      <c r="BX42">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -9398,23 +9526,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057450A-E09F-4265-8443-CBC3C0F00E79}">
   <dimension ref="A1:BG42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="3" width="8.88671875" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>99</v>
       </c>
       <c r="D1">
@@ -9587,13 +9712,13 @@
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2">
@@ -9766,13 +9891,13 @@
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
@@ -9945,13 +10070,13 @@
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>50</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4">
@@ -10124,13 +10249,13 @@
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>204</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5">
@@ -10303,13 +10428,13 @@
       </c>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>854</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6">
@@ -10482,13 +10607,13 @@
       </c>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>108</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7">
@@ -10661,13 +10786,13 @@
       </c>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>116</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8">
@@ -10840,13 +10965,13 @@
       </c>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>120</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9">
@@ -11019,13 +11144,13 @@
       </c>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>384</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10">
@@ -11198,13 +11323,13 @@
       </c>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>180</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11">
@@ -11377,13 +11502,13 @@
       </c>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>818</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
       <c r="D12">
@@ -11556,13 +11681,13 @@
       </c>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>231</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="D13">
@@ -11735,13 +11860,13 @@
       </c>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>288</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
       <c r="D14">
@@ -11914,13 +12039,13 @@
       </c>
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>320</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
       <c r="D15">
@@ -12093,13 +12218,13 @@
       </c>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>324</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>28</v>
       </c>
       <c r="D16">
@@ -12272,13 +12397,13 @@
       </c>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>332</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>29</v>
       </c>
       <c r="D17">
@@ -12451,13 +12576,13 @@
       </c>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>356</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>30</v>
       </c>
       <c r="D18">
@@ -12630,13 +12755,13 @@
       </c>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>400</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>31</v>
       </c>
       <c r="D19">
@@ -12809,13 +12934,13 @@
       </c>
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>404</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>32</v>
       </c>
       <c r="D20">
@@ -12988,13 +13113,13 @@
       </c>
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>430</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>33</v>
       </c>
       <c r="D21">
@@ -13167,13 +13292,13 @@
       </c>
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>450</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>34</v>
       </c>
       <c r="D22">
@@ -13346,13 +13471,13 @@
       </c>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>454</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>35</v>
       </c>
       <c r="D23">
@@ -13525,13 +13650,13 @@
       </c>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>466</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>36</v>
       </c>
       <c r="D24">
@@ -13704,13 +13829,13 @@
       </c>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>478</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>37</v>
       </c>
       <c r="D25">
@@ -13883,13 +14008,13 @@
       </c>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>508</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>38</v>
       </c>
       <c r="D26">
@@ -14062,13 +14187,13 @@
       </c>
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+      <c r="A27">
         <v>524</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>39</v>
       </c>
       <c r="D27">
@@ -14241,13 +14366,13 @@
       </c>
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>562</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>40</v>
       </c>
       <c r="D28">
@@ -14420,13 +14545,13 @@
       </c>
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+      <c r="A29">
         <v>566</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>41</v>
       </c>
       <c r="D29">
@@ -14599,13 +14724,13 @@
       </c>
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+      <c r="A30">
         <v>586</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>42</v>
       </c>
       <c r="D30">
@@ -14778,13 +14903,13 @@
       </c>
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+      <c r="A31">
         <v>608</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>43</v>
       </c>
       <c r="D31">
@@ -14957,13 +15082,13 @@
       </c>
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>646</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>44</v>
       </c>
       <c r="D32">
@@ -15136,13 +15261,13 @@
       </c>
     </row>
     <row r="33" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>686</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>45</v>
       </c>
       <c r="D33">
@@ -15315,13 +15440,13 @@
       </c>
     </row>
     <row r="34" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>694</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>46</v>
       </c>
       <c r="D34">
@@ -15494,13 +15619,13 @@
       </c>
     </row>
     <row r="35" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+      <c r="A35">
         <v>728</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>47</v>
       </c>
       <c r="D35">
@@ -15673,13 +15798,13 @@
       </c>
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>834</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>49</v>
       </c>
       <c r="D36">
@@ -15852,13 +15977,13 @@
       </c>
     </row>
     <row r="37" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>626</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>50</v>
       </c>
       <c r="D37">
@@ -16031,13 +16156,13 @@
       </c>
     </row>
     <row r="38" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+      <c r="A38">
         <v>768</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>51</v>
       </c>
       <c r="D38">
@@ -16210,13 +16335,13 @@
       </c>
     </row>
     <row r="39" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+      <c r="A39">
         <v>800</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>52</v>
       </c>
       <c r="D39">
@@ -16389,13 +16514,13 @@
       </c>
     </row>
     <row r="40" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+      <c r="A40">
         <v>887</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>53</v>
       </c>
       <c r="D40">
@@ -16568,13 +16693,13 @@
       </c>
     </row>
     <row r="41" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+      <c r="A41">
         <v>894</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>54</v>
       </c>
       <c r="D41">
@@ -16747,13 +16872,13 @@
       </c>
     </row>
     <row r="42" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+      <c r="A42">
         <v>716</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>55</v>
       </c>
       <c r="D42">
@@ -16939,18 +17064,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="3" width="8.88671875" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>99</v>
       </c>
       <c r="D1">
@@ -17123,13 +17245,13 @@
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2">
@@ -17302,13 +17424,13 @@
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
@@ -17481,13 +17603,13 @@
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>50</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4">
@@ -17660,13 +17782,13 @@
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>204</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5">
@@ -17839,13 +17961,13 @@
       </c>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>854</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6">
@@ -18018,13 +18140,13 @@
       </c>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>108</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7">
@@ -18197,13 +18319,13 @@
       </c>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>116</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8">
@@ -18376,13 +18498,13 @@
       </c>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>120</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9">
@@ -18555,13 +18677,13 @@
       </c>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>384</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10">
@@ -18734,13 +18856,13 @@
       </c>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>180</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11">
@@ -18913,13 +19035,13 @@
       </c>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>818</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
       <c r="D12">
@@ -19092,13 +19214,13 @@
       </c>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>231</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="D13">
@@ -19271,13 +19393,13 @@
       </c>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>288</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
       <c r="D14">
@@ -19450,13 +19572,13 @@
       </c>
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>320</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
       <c r="D15">
@@ -19629,13 +19751,13 @@
       </c>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>324</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>28</v>
       </c>
       <c r="D16">
@@ -19808,13 +19930,13 @@
       </c>
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>332</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>29</v>
       </c>
       <c r="D17">
@@ -19987,13 +20109,13 @@
       </c>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>356</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>30</v>
       </c>
       <c r="D18">
@@ -20166,13 +20288,13 @@
       </c>
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>400</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>31</v>
       </c>
       <c r="D19">
@@ -20345,13 +20467,13 @@
       </c>
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>404</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>32</v>
       </c>
       <c r="D20">
@@ -20524,13 +20646,13 @@
       </c>
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>430</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>33</v>
       </c>
       <c r="D21">
@@ -20703,13 +20825,13 @@
       </c>
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>450</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>34</v>
       </c>
       <c r="D22">
@@ -20882,13 +21004,13 @@
       </c>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>454</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>35</v>
       </c>
       <c r="D23">
@@ -21061,13 +21183,13 @@
       </c>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>466</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>36</v>
       </c>
       <c r="D24">
@@ -21240,13 +21362,13 @@
       </c>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+      <c r="A25">
         <v>478</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>37</v>
       </c>
       <c r="D25">
@@ -21419,13 +21541,13 @@
       </c>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+      <c r="A26">
         <v>508</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>38</v>
       </c>
       <c r="D26">
@@ -21598,13 +21720,13 @@
       </c>
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+      <c r="A27">
         <v>524</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>39</v>
       </c>
       <c r="D27">
@@ -21777,13 +21899,13 @@
       </c>
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+      <c r="A28">
         <v>562</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>40</v>
       </c>
       <c r="D28">
@@ -21956,13 +22078,13 @@
       </c>
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+      <c r="A29">
         <v>566</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>41</v>
       </c>
       <c r="D29">
@@ -22135,13 +22257,13 @@
       </c>
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+      <c r="A30">
         <v>586</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>42</v>
       </c>
       <c r="D30">
@@ -22314,13 +22436,13 @@
       </c>
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+      <c r="A31">
         <v>608</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>43</v>
       </c>
       <c r="D31">
@@ -22493,13 +22615,13 @@
       </c>
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>646</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>44</v>
       </c>
       <c r="D32">
@@ -22672,13 +22794,13 @@
       </c>
     </row>
     <row r="33" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>686</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>45</v>
       </c>
       <c r="D33">
@@ -22851,13 +22973,13 @@
       </c>
     </row>
     <row r="34" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+      <c r="A34">
         <v>694</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>46</v>
       </c>
       <c r="D34">
@@ -23030,13 +23152,13 @@
       </c>
     </row>
     <row r="35" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+      <c r="A35">
         <v>728</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>47</v>
       </c>
       <c r="D35">
@@ -23209,13 +23331,13 @@
       </c>
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+      <c r="A36">
         <v>834</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>49</v>
       </c>
       <c r="D36">
@@ -23388,13 +23510,13 @@
       </c>
     </row>
     <row r="37" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>626</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>50</v>
       </c>
       <c r="D37">
@@ -23567,13 +23689,13 @@
       </c>
     </row>
     <row r="38" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+      <c r="A38">
         <v>768</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>51</v>
       </c>
       <c r="D38">
@@ -23746,13 +23868,13 @@
       </c>
     </row>
     <row r="39" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+      <c r="A39">
         <v>800</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>52</v>
       </c>
       <c r="D39">
@@ -23925,13 +24047,13 @@
       </c>
     </row>
     <row r="40" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+      <c r="A40">
         <v>887</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>53</v>
       </c>
       <c r="D40">
@@ -24104,13 +24226,13 @@
       </c>
     </row>
     <row r="41" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+      <c r="A41">
         <v>894</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>54</v>
       </c>
       <c r="D41">
@@ -24283,13 +24405,13 @@
       </c>
     </row>
     <row r="42" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+      <c r="A42">
         <v>716</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>55</v>
       </c>
       <c r="D42">

</xml_diff>